<commit_message>
Added NO_FISH to 2016 Baker North
</commit_message>
<xml_diff>
--- a/raw_data/KEEN ONE/Byrnes/2016/Baker North 2016/BakerNorth_fish_2016.xlsx
+++ b/raw_data/KEEN ONE/Byrnes/2016/Baker North 2016/BakerNorth_fish_2016.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="31220" yWindow="-9920" windowWidth="30760" windowHeight="13320"/>
+    <workbookView xWindow="4400" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Data Entry" sheetId="1" r:id="rId1"/>
@@ -194,7 +194,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="145">
   <si>
     <t>YEAR</t>
   </si>
@@ -626,6 +626,9 @@
   </si>
   <si>
     <t>IR</t>
+  </si>
+  <si>
+    <t>NO_FISH</t>
   </si>
 </sst>
 </file>
@@ -1213,7 +1216,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M3" sqref="M3"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1324,7 +1327,7 @@
         <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>78</v>
+        <v>144</v>
       </c>
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>

</xml_diff>